<commit_message>
Detailed Lighting Design. Branch bgm.
</commit_message>
<xml_diff>
--- a/LedLight.xlsx
+++ b/LedLight.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="1180" windowWidth="33180" windowHeight="22200" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3020" yWindow="1180" windowWidth="33180" windowHeight="22200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="30">
   <si>
     <t>//</t>
     <phoneticPr fontId="1"/>
@@ -87,27 +87,67 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>const int NUM_LIGHTS_DYNAMIC = sizeof(Light_Dynamic) / sizeof(Light_Dynamic[0]);</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LED_LIGHT Light_Climax[] = {</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LED_LIGHT Light_Back[] = {</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>const int NUM_LIGHTS_BACK = sizeof(Light_Back) / sizeof(Light_Back[0]);</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>const int NUM_LIGHTS_CLIMAX = sizeof(Light_Climax) / sizeof(Light_Climax[0]);</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>LED_LIGHT Light_Dynamic[] = {</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>const int NUM_LIGHTS_DYNAMIC = sizeof(Light_Dynamic) / sizeof(Light_Dynamic[0]);</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>LED_LIGHT Light_Climax[] = {</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>LED_LIGHT Light_Back[] = {</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>const int NUM_LIGHTS_BACK = sizeof(Light_Back) / sizeof(Light_Back[0]);</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>const int NUM_LIGHTS_CLIMAX = sizeof(Light_Climax) / sizeof(Light_Climax[0]);</t>
+    <t>LED_LIGHT* Light_Dynamic_Eye = &amp;Light_Dynamic[0];</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LED_LIGHT* Light_Dynamic_FaceUp = &amp;Light_Dynamic[1];</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LED_LIGHT* Light_Dynamic_FaceLow = &amp;Light_Dynamic[2];</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LED_LIGHT* Light_Dynamic_ArmUp = &amp;Light_Dynamic[3];</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LED_LIGHT* Light_Dynamic_ArmLow = &amp;Light_Dynamic[4];</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>const int NUM_LIGHTS_EYE = 1;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>const int NUM_LIGHTS_FACE_UP = 1;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>const int NUM_LIGHTS_FACE_LOW = 1;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>const int NUM_LIGHTS_ARM_UP = 1;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>const int NUM_LIGHTS_ARM_LOW = 1;</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -431,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -455,7 +495,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -872,7 +912,57 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -885,7 +975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -907,7 +997,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1129,7 +1219,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1164,7 +1254,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1386,7 +1476,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>